<commit_message>
linux managed systemler ok
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EnesPekdas\Desktop\Projeler\BT-THY\Otomasyon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22582AE-C64F-4495-9C07-C4F632C5E8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDB5CB1-B6A3-47D3-8AD4-18B9CB47E75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-240" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>Target system address</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>standby1.quasys.local</t>
+  </si>
+  <si>
+    <t>standby3.quasys.locals</t>
+  </si>
+  <si>
+    <t>bastion.quasys.local</t>
   </si>
 </sst>
 </file>
@@ -508,7 +514,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -612,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
@@ -684,7 +690,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
ad hesapları ok , local hesaplara geçiliyor
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EnesPekdas\Desktop\Projeler\BT-THY\Otomasyon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDB5CB1-B6A3-47D3-8AD4-18B9CB47E75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB61ED5B-A609-47B7-88A1-0D956901072A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-240" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Target system address</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>bastion.quasys.local</t>
+  </si>
+  <si>
+    <t>pam118065</t>
   </si>
 </sst>
 </file>
@@ -514,7 +517,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -599,7 +602,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>35</v>

</xml_diff>